<commit_message>
Regenerated outputs for following IG's which has got an update to their CDA IG's - Advanced Care Records - Event Summary - Personal Health Records - Prescription Dispense Lists - Shared Health Summary
CIFMM-2527
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/organization-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/organization-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4151" uniqueCount="384">
   <si>
     <t>Path</t>
   </si>
@@ -1142,19 +1142,33 @@
 </t>
   </si>
   <si>
-    <t>A name associated with the contact</t>
-  </si>
-  <si>
-    <t>A name associated with the contact.</t>
+    <t>Name of a human - parts and usage</t>
+  </si>
+  <si>
+    <t>A human's name with the ability to identify parts and usage.</t>
+  </si>
+  <si>
+    <t>Names may be changed, or repudiated, or people may have different names in different contexts. Names may be divided into parts of different type that have variable significance depending on context, though the division into parts does not always matter. With personal names, the different parts may or may not be imbued with some implicit meaning; various cultures associate different importance with the name parts and the degree to which systems must care about name parts around the world varies widely.</t>
   </si>
   <si>
     <t>Need to be able to track the person by name.</t>
   </si>
   <si>
-    <t>PID-5, PID-9</t>
-  </si>
-  <si>
-    <t>./name</t>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+inv-dh-humn-01:The name shall at least have text or a family name or a given name {text.exists() or family.exists() or given.exists()}</t>
+  </si>
+  <si>
+    <t>XPN</t>
+  </si>
+  <si>
+    <t>EN (actually, PN)</t>
+  </si>
+  <si>
+    <t>ProviderName</t>
   </si>
   <si>
     <t>Organization.contact.telecom</t>
@@ -14132,9 +14146,11 @@
       <c r="L115" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="M115" s="2"/>
+      <c r="M115" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="N115" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="O115" t="s" s="2">
         <v>40</v>
@@ -14192,19 +14208,19 @@
         <v>50</v>
       </c>
       <c r="AH115" t="s" s="2">
-        <v>40</v>
+        <v>362</v>
       </c>
       <c r="AI115" t="s" s="2">
-        <v>40</v>
+        <v>363</v>
       </c>
       <c r="AJ115" t="s" s="2">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="AK115" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AL115" t="s" s="2">
-        <v>40</v>
+        <v>366</v>
       </c>
       <c r="AM115" t="s" s="2">
         <v>40</v>
@@ -14212,7 +14228,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" t="s" s="2">
@@ -14238,14 +14254,14 @@
         <v>308</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" t="s" s="2">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="O116" t="s" s="2">
         <v>40</v>
@@ -14294,7 +14310,7 @@
         <v>40</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>41</v>
@@ -14309,10 +14325,10 @@
         <v>40</v>
       </c>
       <c r="AJ116" t="s" s="2">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="AK116" t="s" s="2">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="AL116" t="s" s="2">
         <v>40</v>
@@ -14323,7 +14339,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -14349,14 +14365,14 @@
         <v>319</v>
       </c>
       <c r="K117" t="s" s="2">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="M117" s="2"/>
       <c r="N117" t="s" s="2">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="O117" t="s" s="2">
         <v>40</v>
@@ -14405,7 +14421,7 @@
         <v>40</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>41</v>
@@ -14420,10 +14436,10 @@
         <v>40</v>
       </c>
       <c r="AJ117" t="s" s="2">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="AK117" t="s" s="2">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="AL117" t="s" s="2">
         <v>40</v>
@@ -14434,7 +14450,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -14457,17 +14473,17 @@
         <v>40</v>
       </c>
       <c r="J118" t="s" s="2">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="M118" s="2"/>
       <c r="N118" t="s" s="2">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="O118" t="s" s="2">
         <v>40</v>
@@ -14516,7 +14532,7 @@
         <v>40</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>41</v>

</xml_diff>